<commit_message>
added 3 csvs containing the final data, including a has_comorbs column (0=no, 1=yes)
</commit_message>
<xml_diff>
--- a/data/column_lookups.xlsx
+++ b/data/column_lookups.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_6F9903F16A438B3BC12D4CF8ED6F3A9379780F2D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A28933CA-5588-3B4B-99BA-0AB4B738B5E0}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d64c27655461cefb/project/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_6F9903F16A438B3BC12D4CF8ED6F3A9379780F2D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C86CC6A3-6AB3-481C-A216-6FD66B8BFA0C}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24400" yWindow="2700" windowWidth="21160" windowHeight="15490" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="346">
   <si>
     <t>study_id</t>
   </si>
@@ -1467,16 +1473,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C174"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="B160" activeCellId="23" sqref="B2 B10 B11 B13 B26 B27 B41 B54 B57 B63 B64 B76 B95 B96 B97 B98 B99 B100 B129 B130 B131 B132 B133 B160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="27.3046875" customWidth="1"/>
+    <col min="2" max="2" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -1484,7 +1490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1495,7 +1501,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1506,7 +1512,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1517,7 +1523,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1528,7 +1534,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1539,7 +1545,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1550,7 +1556,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1561,7 +1567,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1572,7 +1578,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1583,7 +1589,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1594,7 +1600,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1605,7 +1611,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1616,7 +1622,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1627,7 +1633,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1638,7 +1644,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1649,7 +1655,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1660,7 +1666,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1671,7 +1677,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1682,7 +1688,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1693,7 +1699,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1704,7 +1710,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1715,7 +1721,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1726,7 +1732,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1737,7 +1743,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1748,7 +1754,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1759,7 +1765,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1770,7 +1776,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1781,7 +1787,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1792,7 +1798,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1803,7 +1809,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1814,7 +1820,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1825,7 +1831,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1836,7 +1842,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1847,7 +1853,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1858,7 +1864,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1869,7 +1875,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1880,7 +1886,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1891,7 +1897,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1902,7 +1908,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1913,7 +1919,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1924,7 +1930,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1935,7 +1941,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1946,7 +1952,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1957,7 +1963,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1968,7 +1974,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1979,7 +1985,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1990,7 +1996,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2001,7 +2007,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2012,7 +2018,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2023,7 +2029,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2034,7 +2040,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2045,7 +2051,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2056,7 +2062,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2067,7 +2073,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2078,7 +2084,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2089,7 +2095,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2100,7 +2106,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2111,7 +2117,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2122,7 +2128,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2133,7 +2139,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2144,7 +2150,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2155,7 +2161,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2166,7 +2172,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2177,7 +2183,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2188,7 +2194,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2199,7 +2205,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2210,7 +2216,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2221,7 +2227,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2232,7 +2238,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2243,7 +2249,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2254,7 +2260,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2265,7 +2271,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2276,7 +2282,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2287,7 +2293,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2298,7 +2304,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2309,7 +2315,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2320,7 +2326,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2331,7 +2337,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2342,7 +2348,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2353,7 +2359,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2364,7 +2370,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2375,7 +2381,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2386,7 +2392,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2397,7 +2403,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2408,7 +2414,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2419,7 +2425,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2430,7 +2436,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2441,7 +2447,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2452,7 +2458,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2463,7 +2469,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2474,7 +2480,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2485,7 +2491,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2496,7 +2502,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2507,7 +2513,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2518,7 +2524,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2529,7 +2535,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -2540,7 +2546,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2551,7 +2557,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -2562,7 +2568,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -2573,7 +2579,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -2584,7 +2590,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2595,7 +2601,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -2606,7 +2612,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -2617,7 +2623,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -2628,7 +2634,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -2639,7 +2645,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -2650,7 +2656,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -2661,7 +2667,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -2672,7 +2678,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -2683,7 +2689,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -2694,7 +2700,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -2705,7 +2711,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -2716,7 +2722,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -2727,7 +2733,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -2738,7 +2744,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -2749,7 +2755,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -2760,7 +2766,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -2771,7 +2777,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -2782,7 +2788,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -2793,7 +2799,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -2804,7 +2810,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -2815,7 +2821,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -2826,7 +2832,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -2837,7 +2843,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -2848,7 +2854,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -2859,7 +2865,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -2870,7 +2876,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -2881,7 +2887,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -2892,7 +2898,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -2903,7 +2909,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -2914,7 +2920,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -2925,7 +2931,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -2936,7 +2942,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -2947,7 +2953,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -2958,7 +2964,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -2969,7 +2975,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -2980,7 +2986,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -2991,7 +2997,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -3002,7 +3008,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -3013,7 +3019,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -3024,7 +3030,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -3035,7 +3041,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -3046,7 +3052,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -3057,7 +3063,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -3068,7 +3074,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -3079,7 +3085,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -3090,7 +3096,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -3101,7 +3107,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -3112,7 +3118,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -3134,7 +3140,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -3145,7 +3151,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -3156,7 +3162,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -3167,7 +3173,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -3178,7 +3184,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -3189,7 +3195,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -3200,7 +3206,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -3211,7 +3217,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -3222,7 +3228,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -3233,7 +3239,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -3244,7 +3250,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -3255,7 +3261,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -3266,7 +3272,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -3277,7 +3283,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -3288,7 +3294,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -3299,7 +3305,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -3310,7 +3316,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -3321,7 +3327,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -3332,7 +3338,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -3343,7 +3349,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -3354,7 +3360,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -3365,7 +3371,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -3376,7 +3382,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -3385,6 +3391,141 @@
       </c>
       <c r="C174" t="s">
         <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EE8D5B3-195D-4651-933C-333FE9C9FB6E}">
+  <dimension ref="A1:A24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>